<commit_message>
second commit "Excluisão do funcionário Igor"
</commit_message>
<xml_diff>
--- a/dataset/banco_nomes.xlsx
+++ b/dataset/banco_nomes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">CPF</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">GUILHERME MARTINS JORDÃO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IGOR CESAR FIOREZI TEIXEIRA</t>
   </si>
   <si>
     <t xml:space="preserve">ISABELLA REGINA DE OLIVEIRA CALLE</t>
@@ -193,6 +190,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -259,12 +257,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,577 +287,566 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="47.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>30096013877</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>12718701171</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>37823890852</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>20492160354</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>42213740801</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>12580820827</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>45989810830</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>21044371287</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>43733679814</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>14553150294</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>43174865808</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>20151030213</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>43968845838</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <v>16137733603</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>40881056804</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <v>16177359621</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <v>22380873895</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="2" t="n">
         <v>12591774163</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>16186760839</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="2" t="n">
         <v>12490886934</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>36183207870</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="2" t="n">
         <v>13792453818</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <v>48478361898</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="2" t="n">
         <v>26782938934</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>34548193855</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="2" t="n">
         <v>12887931182</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <v>43844679820</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="2" t="n">
         <v>20492148877</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="2" t="n">
         <v>47912071814</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="2" t="n">
         <v>20664231262</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="2" t="n">
         <v>44391468808</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="2" t="n">
         <v>20097423062</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="2" t="n">
         <v>22510736809</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" s="2" t="n">
         <v>12728471160</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="2" t="n">
         <v>42419173805</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="2" t="n">
         <v>20216146431</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="2" t="n">
         <v>43010710836</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" s="2" t="n">
         <v>14020178913</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="2" t="n">
         <v>39475546804</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="2" t="n">
         <v>12971142142</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>47925371854</v>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>20165327124</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="A22" s="2" t="n">
+        <v>50086064843</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>23719827417</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>50086064843</v>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>23719827417</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="A23" s="2" t="n">
+        <v>22945036860</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>12845610183</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>22945036860</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>12845610183</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="A24" s="2" t="n">
+        <v>26813914820</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>12733417152</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>26813914820</v>
-      </c>
-      <c r="B25" s="1" t="n">
-        <v>12733417152</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="A25" s="2" t="n">
+        <v>30842206892</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>13517103534</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
-        <v>30842206892</v>
-      </c>
-      <c r="B26" s="1" t="n">
-        <v>13517103534</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="A26" s="2" t="n">
+        <v>48995670819</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>16506582341</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
-        <v>48995670819</v>
-      </c>
-      <c r="B27" s="1" t="n">
-        <v>16506582341</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="A27" s="2" t="n">
+        <v>44163433880</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>20326138050</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>44163433880</v>
-      </c>
-      <c r="B28" s="1" t="n">
-        <v>20326138050</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="A28" s="2" t="n">
+        <v>43558459822</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>16484578126</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>43558459822</v>
-      </c>
-      <c r="B29" s="1" t="n">
-        <v>16484578126</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="A29" s="2" t="n">
+        <v>26709794830</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>12933332177</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>26709794830</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>12933332177</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="A30" s="2" t="n">
+        <v>42534730835</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>20664251263</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>42534730835</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>20664251263</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="A31" s="2" t="n">
+        <v>41375946862</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>27038366373</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>41375946862</v>
-      </c>
-      <c r="B32" s="1" t="n">
-        <v>27038366373</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="A32" s="2" t="n">
+        <v>26597530837</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>12514750867</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>26597530837</v>
-      </c>
-      <c r="B33" s="1" t="n">
-        <v>12514750867</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="A33" s="2" t="n">
+        <v>44138766871</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>12587060747</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>44138766871</v>
-      </c>
-      <c r="B34" s="1" t="n">
-        <v>12587060747</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="A34" s="2" t="n">
+        <v>28056157867</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>20663779744</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>28056157867</v>
-      </c>
-      <c r="B35" s="1" t="n">
-        <v>20663779744</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="A35" s="2" t="n">
+        <v>45115153874</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>13409206298</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>45115153874</v>
-      </c>
-      <c r="B36" s="1" t="n">
-        <v>13409206298</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="A36" s="2" t="n">
+        <v>9636891850</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>12808296160</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>9636891850</v>
-      </c>
-      <c r="B37" s="1" t="n">
-        <v>12808296160</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="A37" s="2" t="n">
+        <v>44081141894</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>16447113875</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>44081141894</v>
-      </c>
-      <c r="B38" s="1" t="n">
-        <v>16447113875</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="A38" s="2" t="n">
+        <v>46537913845</v>
+      </c>
+      <c r="B38" s="2" t="n">
+        <v>14715452347</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
-        <v>46537913845</v>
-      </c>
-      <c r="B39" s="1" t="n">
-        <v>14715452347</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="A39" s="2" t="n">
+        <v>46115095832</v>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>16596352057</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>46115095832</v>
-      </c>
-      <c r="B40" s="1" t="n">
-        <v>16596352057</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="A40" s="2" t="n">
+        <v>43343943886</v>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>16615667151</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>43343943886</v>
-      </c>
-      <c r="B41" s="1" t="n">
-        <v>16615667151</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="A41" s="2" t="n">
+        <v>35991462844</v>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>16550107653</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>35991462844</v>
-      </c>
-      <c r="B42" s="1" t="n">
-        <v>16550107653</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="A42" s="2" t="n">
+        <v>51637097808</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>20330845068</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>51637097808</v>
-      </c>
-      <c r="B43" s="1" t="n">
-        <v>20330845068</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="A43" s="2" t="n">
+        <v>45517749879</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>16663672860</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>45517749879</v>
-      </c>
-      <c r="B44" s="1" t="n">
-        <v>16663672860</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="A44" s="2" t="n">
+        <v>40165587865</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>20650402892</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <v>40165587865</v>
-      </c>
-      <c r="B45" s="1" t="n">
-        <v>20650402892</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="A45" s="2" t="n">
+        <v>31942788860</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>12809605159</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
-        <v>31942788860</v>
-      </c>
-      <c r="B46" s="1" t="n">
-        <v>12809605159</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="A46" s="2" t="n">
+        <v>40952721805</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>20121609582</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
-        <v>40952721805</v>
-      </c>
-      <c r="B47" s="1" t="n">
-        <v>20121609582</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="A47" s="2" t="n">
+        <v>21841129844</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>12646787164</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>21841129844</v>
-      </c>
-      <c r="B48" s="1" t="n">
-        <v>12646787164</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="A48" s="2" t="n">
+        <v>22148871803</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>12723612165</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>22148871803</v>
-      </c>
-      <c r="B49" s="1" t="n">
-        <v>12723612165</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="A49" s="2" t="n">
+        <v>42421185890</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>15567916160</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <v>42421185890</v>
-      </c>
-      <c r="B50" s="1" t="n">
-        <v>15567916160</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="A50" s="2" t="n">
+        <v>51099482838</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>20694654994</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
-        <v>51099482838</v>
-      </c>
-      <c r="B51" s="1" t="n">
-        <v>20694654994</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
second commit "exclusão do colaborador Fabio"
</commit_message>
<xml_diff>
--- a/dataset/banco_nomes.xlsx
+++ b/dataset/banco_nomes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">CPF</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">CHRISTIANE GRADIM FERREIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FABIO FIGUEIRO MACHIDA</t>
   </si>
   <si>
     <t xml:space="preserve">FELIPE BARBOZA ROCHA DA SILVA</t>
@@ -287,10 +284,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -422,10 +419,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
-        <v>36183207870</v>
+        <v>48478361898</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>13792453818</v>
+        <v>26782938934</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>13</v>
@@ -433,10 +430,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
-        <v>48478361898</v>
+        <v>34548193855</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>26782938934</v>
+        <v>12887931182</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>14</v>
@@ -444,10 +441,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
-        <v>34548193855</v>
+        <v>43844679820</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>12887931182</v>
+        <v>20492148877</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
@@ -455,10 +452,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>43844679820</v>
+        <v>47912071814</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>20492148877</v>
+        <v>20664231262</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
@@ -466,10 +463,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>47912071814</v>
+        <v>44391468808</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>20664231262</v>
+        <v>20097423062</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
@@ -477,10 +474,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>44391468808</v>
+        <v>22510736809</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>20097423062</v>
+        <v>12728471160</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -488,10 +485,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
-        <v>22510736809</v>
+        <v>42419173805</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>12728471160</v>
+        <v>20216146431</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>19</v>
@@ -499,10 +496,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
-        <v>42419173805</v>
+        <v>43010710836</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>20216146431</v>
+        <v>14020178913</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>20</v>
@@ -510,10 +507,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
-        <v>43010710836</v>
+        <v>39475546804</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>14020178913</v>
+        <v>12971142142</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
@@ -521,10 +518,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
-        <v>39475546804</v>
+        <v>50086064843</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>12971142142</v>
+        <v>23719827417</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>22</v>
@@ -532,10 +529,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
-        <v>50086064843</v>
+        <v>22945036860</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>23719827417</v>
+        <v>12845610183</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>23</v>
@@ -543,10 +540,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
-        <v>22945036860</v>
+        <v>26813914820</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>12845610183</v>
+        <v>12733417152</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>24</v>
@@ -554,10 +551,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
-        <v>26813914820</v>
+        <v>30842206892</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>12733417152</v>
+        <v>13517103534</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>25</v>
@@ -565,10 +562,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
-        <v>30842206892</v>
+        <v>48995670819</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>13517103534</v>
+        <v>16506582341</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>26</v>
@@ -576,10 +573,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
-        <v>48995670819</v>
+        <v>44163433880</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>16506582341</v>
+        <v>20326138050</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>27</v>
@@ -587,10 +584,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
-        <v>44163433880</v>
+        <v>43558459822</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>20326138050</v>
+        <v>16484578126</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>28</v>
@@ -598,10 +595,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
-        <v>43558459822</v>
+        <v>26709794830</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>16484578126</v>
+        <v>12933332177</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>29</v>
@@ -609,10 +606,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
-        <v>26709794830</v>
+        <v>42534730835</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>12933332177</v>
+        <v>20664251263</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>30</v>
@@ -620,10 +617,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
-        <v>42534730835</v>
+        <v>41375946862</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>20664251263</v>
+        <v>27038366373</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>31</v>
@@ -631,10 +628,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
-        <v>41375946862</v>
+        <v>26597530837</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>27038366373</v>
+        <v>12514750867</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>32</v>
@@ -642,10 +639,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
-        <v>26597530837</v>
+        <v>44138766871</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>12514750867</v>
+        <v>12587060747</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>33</v>
@@ -653,10 +650,10 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
-        <v>44138766871</v>
+        <v>28056157867</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>12587060747</v>
+        <v>20663779744</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>34</v>
@@ -664,10 +661,10 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
-        <v>28056157867</v>
+        <v>45115153874</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>20663779744</v>
+        <v>13409206298</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>35</v>
@@ -675,10 +672,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
-        <v>45115153874</v>
+        <v>9636891850</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>13409206298</v>
+        <v>12808296160</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>36</v>
@@ -686,10 +683,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
-        <v>9636891850</v>
+        <v>44081141894</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>12808296160</v>
+        <v>16447113875</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>37</v>
@@ -697,10 +694,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
-        <v>44081141894</v>
+        <v>46537913845</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>16447113875</v>
+        <v>14715452347</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>38</v>
@@ -708,10 +705,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
-        <v>46537913845</v>
+        <v>46115095832</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>14715452347</v>
+        <v>16596352057</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>39</v>
@@ -719,10 +716,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
-        <v>46115095832</v>
+        <v>43343943886</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>16596352057</v>
+        <v>16615667151</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>40</v>
@@ -730,10 +727,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
-        <v>43343943886</v>
+        <v>35991462844</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>16615667151</v>
+        <v>16550107653</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>41</v>
@@ -741,10 +738,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
-        <v>35991462844</v>
+        <v>51637097808</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>16550107653</v>
+        <v>20330845068</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>42</v>
@@ -752,10 +749,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
-        <v>51637097808</v>
+        <v>45517749879</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>20330845068</v>
+        <v>16663672860</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>43</v>
@@ -763,10 +760,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
-        <v>45517749879</v>
+        <v>40165587865</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>16663672860</v>
+        <v>20650402892</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>44</v>
@@ -774,10 +771,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
-        <v>40165587865</v>
+        <v>31942788860</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>20650402892</v>
+        <v>12809605159</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>45</v>
@@ -785,10 +782,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
-        <v>31942788860</v>
+        <v>40952721805</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>12809605159</v>
+        <v>20121609582</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>46</v>
@@ -796,10 +793,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
-        <v>40952721805</v>
+        <v>21841129844</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>20121609582</v>
+        <v>12646787164</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>47</v>
@@ -807,10 +804,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
-        <v>21841129844</v>
+        <v>22148871803</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>12646787164</v>
+        <v>12723612165</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -818,10 +815,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
-        <v>22148871803</v>
+        <v>42421185890</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>12723612165</v>
+        <v>15567916160</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>49</v>
@@ -829,24 +826,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
-        <v>42421185890</v>
+        <v>51099482838</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>15567916160</v>
+        <v>20694654994</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="n">
-        <v>51099482838</v>
-      </c>
-      <c r="B50" s="2" t="n">
-        <v>20694654994</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thrid commit "exclusão/inclusão de funcionarios "
</commit_message>
<xml_diff>
--- a/dataset/banco_nomes.xlsx
+++ b/dataset/banco_nomes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">CPF</t>
   </si>
@@ -163,9 +163,6 @@
     <t xml:space="preserve">VILMA TAMIOSO</t>
   </si>
   <si>
-    <t xml:space="preserve">VIVIAN CRISTINA DOS SANTOS RAMOS</t>
-  </si>
-  <si>
     <t xml:space="preserve">VIVIANE CORREA DAS CHAGAS</t>
   </si>
   <si>
@@ -173,6 +170,15 @@
   </si>
   <si>
     <t xml:space="preserve">GABRIEL JUNIOR DE PAULA FIDENCIO DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEONARDO JUNIOR GODOY FERREIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GABRIEL DE SOUZA TAHARA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANA CAROLINE DE ARAUJO DE OLIVEIRA</t>
   </si>
 </sst>
 </file>
@@ -254,7 +260,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,6 +270,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -284,10 +294,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -793,10 +803,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
-        <v>21841129844</v>
+        <v>22148871803</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>12646787164</v>
+        <v>12723612165</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>47</v>
@@ -804,10 +814,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
-        <v>22148871803</v>
+        <v>42421185890</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>12723612165</v>
+        <v>15567916160</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -815,24 +825,46 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
-        <v>42421185890</v>
+        <v>51099482838</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>15567916160</v>
+        <v>20694654994</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="n">
-        <v>51099482838</v>
-      </c>
-      <c r="B49" s="2" t="n">
-        <v>20694654994</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="A49" s="3" t="n">
+        <v>33200877898</v>
+      </c>
+      <c r="B49" s="3" t="n">
+        <v>20492142968</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="n">
+        <v>45243244880</v>
+      </c>
+      <c r="B50" s="3" t="n">
+        <v>21301771017</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="n">
+        <v>31981527800</v>
+      </c>
+      <c r="B51" s="3" t="n">
+        <v>12868348434</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fifth commit "Inclusão de CASSIA SILVA"
</commit_message>
<xml_diff>
--- a/dataset/banco_nomes.xlsx
+++ b/dataset/banco_nomes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiomachida/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.machida\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6044DAA-A4FD-2F42-8AFC-A03090BC8293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC93EF4E-3779-4871-A065-A787D9C1BE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>CPF</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>BRENDA EDUARDA AMANCIO DE PAULO</t>
+  </si>
+  <si>
+    <t>CASSIA PEREIRA MARQUES DA SILVA</t>
   </si>
 </sst>
 </file>
@@ -582,19 +585,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="242" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:C56"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="1" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>30096013877</v>
       </c>
@@ -616,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>37823890852</v>
       </c>
@@ -627,7 +630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42213740801</v>
       </c>
@@ -638,7 +641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45989810830</v>
       </c>
@@ -649,7 +652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43733679814</v>
       </c>
@@ -660,7 +663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43174865808</v>
       </c>
@@ -671,7 +674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43968845838</v>
       </c>
@@ -682,7 +685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>40881056804</v>
       </c>
@@ -693,7 +696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>22380873895</v>
       </c>
@@ -704,7 +707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>16186760839</v>
       </c>
@@ -715,7 +718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>48478361898</v>
       </c>
@@ -726,7 +729,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>34548193855</v>
       </c>
@@ -737,7 +740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43844679820</v>
       </c>
@@ -748,7 +751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>47912071814</v>
       </c>
@@ -759,7 +762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44391468808</v>
       </c>
@@ -770,7 +773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>22510736809</v>
       </c>
@@ -781,7 +784,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>42419173805</v>
       </c>
@@ -792,7 +795,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43010710836</v>
       </c>
@@ -803,7 +806,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>39475546804</v>
       </c>
@@ -814,7 +817,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>50086064843</v>
       </c>
@@ -825,7 +828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>22945036860</v>
       </c>
@@ -836,7 +839,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>26813914820</v>
       </c>
@@ -847,7 +850,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>30842206892</v>
       </c>
@@ -858,7 +861,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>48995670819</v>
       </c>
@@ -869,7 +872,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44163433880</v>
       </c>
@@ -880,7 +883,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43558459822</v>
       </c>
@@ -891,7 +894,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26709794830</v>
       </c>
@@ -902,7 +905,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>42534730835</v>
       </c>
@@ -913,7 +916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>41375946862</v>
       </c>
@@ -924,7 +927,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>26597530837</v>
       </c>
@@ -935,7 +938,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44138766871</v>
       </c>
@@ -946,7 +949,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>28056157867</v>
       </c>
@@ -957,7 +960,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>45115153874</v>
       </c>
@@ -968,7 +971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>9636891850</v>
       </c>
@@ -979,7 +982,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>44081141894</v>
       </c>
@@ -990,7 +993,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>46537913845</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>46115095832</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43343943886</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>35991462844</v>
       </c>
@@ -1034,7 +1037,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>51637097808</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>45517749879</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>40165587865</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>31942788860</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>40952721805</v>
       </c>
@@ -1089,7 +1092,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>22148871803</v>
       </c>
@@ -1100,7 +1103,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>42421185890</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>51099482838</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>33200877898</v>
       </c>
@@ -1133,7 +1136,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>45243244880</v>
       </c>
@@ -1144,7 +1147,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>31981527800</v>
       </c>
@@ -1155,7 +1158,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>46137027805</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>46580411899</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>48464442874</v>
       </c>
@@ -1188,7 +1191,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>48433884832</v>
       </c>
@@ -1199,7 +1202,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>42458301827</v>
       </c>
@@ -1208,6 +1211,17 @@
       </c>
       <c r="C56" s="1" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>52561493857</v>
+      </c>
+      <c r="B57" s="1">
+        <v>20440736743</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sixth commit "Ajuste do PIS da colaboradora"
</commit_message>
<xml_diff>
--- a/dataset/banco_nomes.xlsx
+++ b/dataset/banco_nomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.machida\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC93EF4E-3779-4871-A065-A787D9C1BE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C86879-855E-4153-8228-B83F4B3FC933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1196,7 +1196,7 @@
         <v>48433884832</v>
       </c>
       <c r="B55" s="1">
-        <v>21216652394</v>
+        <v>26784791078</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>56</v>

</xml_diff>